<commit_message>
use espn api for roster
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NBA_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD542A85-F3F1-4F3C-A3EC-F12001CD6E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8CEA77-8F87-41E5-BFBA-60EE2336FF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chrome_ver" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="remove" sheetId="2" r:id="rId3"/>
     <sheet name="url" sheetId="5" r:id="rId4"/>
     <sheet name="scrape_call" sheetId="6" r:id="rId5"/>
+    <sheet name="espn_api" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
   <si>
     <t>num</t>
   </si>
@@ -344,6 +345,24 @@
   </si>
   <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>swid</t>
+  </si>
+  <si>
+    <t>espn_s2</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>league_id</t>
+  </si>
+  <si>
+    <t>{1AFA2BA9-0A5B-499B-BC41-CA32FDB46E50}</t>
+  </si>
+  <si>
+    <t>AEB9IogDihpmnSBySa1Dt%2BBZGNCwhpyrx1lOauwtvC2Zk4%2F1%2FXPWx%2BBr2HCsUsK3IL3Y6ansGgILWrmKQ5KG3em296twmYEMjOUDGa%2FwYNQ44GBlps9n6Vtts4%2Fh43ivZJzUzMH6dK5%2BQTwyG4wOoj6hXAjyq6gtHh5qSUDJDxqmeaCejF%2BntpFFHdx5kTfcE46%2F0XnWu7IAW2svLYPC53uMQPeYyBkNwMVfOincdbVpgcbquuF898mZeOnWG8ZjbI4e6Wg9q403IYw5o9ua%2FFk5uRCnpit%2FB9x7zgCmOsmhhA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -693,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1598,4 +1617,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A9F646-F43D-4142-AE84-17444D6F5F85}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2023</v>
+      </c>
+      <c r="B2">
+        <v>44419657</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>